<commit_message>
(#51) Alterando a aplicação para receber uma lista de paths
Co-authored-by: Leandro Silva <Leanddro13@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/exemplo/exemplo.xlsx
+++ b/docs/exemplo/exemplo.xlsx
@@ -144,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,9 +166,6 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -486,8 +483,8 @@
   <cols>
     <col min="1" max="1" style="8" width="21.14785714285714" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="8" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5">
@@ -504,7 +501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -518,7 +515,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -532,7 +529,7 @@
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -546,7 +543,7 @@
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -560,7 +557,7 @@
         <v>75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
@@ -574,7 +571,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
@@ -588,7 +585,7 @@
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -602,7 +599,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="6" t="s">
         <v>21</v>
       </c>

</xml_diff>